<commit_message>
couple new books here
</commit_message>
<xml_diff>
--- a/Readinglist.xlsx
+++ b/Readinglist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Egor\Desktop\lists\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4616DE5-B44B-4E05-967F-B535567C7D69}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72A856FB-9FDC-4D63-B5F7-555F362E1C3A}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{30A61FED-7E5A-4752-B883-7E48605B2873}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="63">
   <si>
     <t>Приоритет</t>
   </si>
@@ -211,7 +211,16 @@
     <t>Marty Cagan</t>
   </si>
   <si>
-    <t>ffff</t>
+    <t>Rich Dad Poor Dad</t>
+  </si>
+  <si>
+    <t>Robert Kiyosaki</t>
+  </si>
+  <si>
+    <t>The Richest Man in Babylon</t>
+  </si>
+  <si>
+    <t>George Samuel Clason</t>
   </si>
 </sst>
 </file>
@@ -595,7 +604,7 @@
   <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -975,9 +984,32 @@
         <v>53</v>
       </c>
     </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>59</v>
+      </c>
+      <c r="B27" t="s">
+        <v>60</v>
+      </c>
+      <c r="C27" t="s">
+        <v>12</v>
+      </c>
+      <c r="F27" t="s">
+        <v>53</v>
+      </c>
+    </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>61</v>
+      </c>
       <c r="B28" t="s">
-        <v>59</v>
+        <v>62</v>
+      </c>
+      <c r="C28" t="s">
+        <v>12</v>
+      </c>
+      <c r="F28" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>